<commit_message>
Cheat sheet version 1.0.0 from acoptex.lt
</commit_message>
<xml_diff>
--- a/Csharp-cheatsheet-acoptexlt.xlsx
+++ b/Csharp-cheatsheet-acoptexlt.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Strings" sheetId="3" r:id="rId2"/>
     <sheet name="Data-structures" sheetId="4" r:id="rId3"/>
     <sheet name="Loops Conditions Ternary operat" sheetId="5" r:id="rId4"/>
+    <sheet name="Links" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913" calcMode="autoNoTable"/>
   <extLst>
@@ -21,8 +22,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="B22" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Acoptex:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+A floating point number can also be a scientific number with an "e" to indicate the power of 10:</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="164">
   <si>
     <t>string.Equals("Text")</t>
   </si>
@@ -96,45 +131,21 @@
     <t>uint</t>
   </si>
   <si>
-    <t>(double)myFloat</t>
-  </si>
-  <si>
-    <t>float-&gt;double</t>
-  </si>
-  <si>
     <t>long</t>
   </si>
   <si>
-    <t>(long)myInt</t>
-  </si>
-  <si>
-    <t>int-&gt;long</t>
-  </si>
-  <si>
     <t>int</t>
   </si>
   <si>
-    <t>Implicit conversion</t>
-  </si>
-  <si>
     <t>byte</t>
   </si>
   <si>
     <t>sbyte</t>
   </si>
   <si>
-    <t>(int)myDouble</t>
-  </si>
-  <si>
-    <t>double-&gt;int</t>
-  </si>
-  <si>
     <t>ushort</t>
   </si>
   <si>
-    <t>Explicit conversion</t>
-  </si>
-  <si>
     <t>short</t>
   </si>
   <si>
@@ -150,24 +161,12 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Single line</t>
-  </si>
-  <si>
-    <t>Multiline</t>
-  </si>
-  <si>
-    <t>Csharp Cheat Sheet version 0.1</t>
-  </si>
-  <si>
     <t>Learn Csharp with Acoptex: https://acoptex.lt</t>
   </si>
   <si>
     <t>Constants</t>
   </si>
   <si>
-    <t>const PI = 3.141569</t>
-  </si>
-  <si>
     <t>Escape Characters</t>
   </si>
   <si>
@@ -533,9 +532,6 @@
     </r>
   </si>
   <si>
-    <t>"text1"+"text2"</t>
-  </si>
-  <si>
     <t>String concatination</t>
   </si>
   <si>
@@ -591,13 +587,480 @@
   </si>
   <si>
     <t>a/b</t>
+  </si>
+  <si>
+    <r>
+      <t>using</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> System</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>namespace</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HelloWorld</t>
+    </r>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0077AA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFDD4A68"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Program</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0077AA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>static</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0077AA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>void</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFDD4A68"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Main</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0077AA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> args</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      Console</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFDD4A68"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>WriteLine</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF669900"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Hello World!"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>https://www.tutorialspoint.com/compile_csharp_online.php</t>
+  </si>
+  <si>
+    <t>https://www.onlinegdb.com/online_csharp_compiler</t>
+  </si>
+  <si>
+    <t>https://www.jdoodle.com/compile-c-sharp-online/</t>
+  </si>
+  <si>
+    <t>https://dotnetfiddle.net/</t>
+  </si>
+  <si>
+    <t>Online Csharp compilers</t>
+  </si>
+  <si>
+    <t>https://www.programiz.com/csharp-programming/online-compiler/</t>
+  </si>
+  <si>
+    <t>https://www.mycompiler.io/new/csharp</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/cs/cs_compiler.php</t>
+  </si>
+  <si>
+    <t>Csharp Cheat Sheet version 1.0.0</t>
+  </si>
+  <si>
+    <t>Console class methods</t>
+  </si>
+  <si>
+    <t>WriteLine('Test')</t>
+  </si>
+  <si>
+    <t>Write('Text')</t>
+  </si>
+  <si>
+    <t>To output values or print text in C#</t>
+  </si>
+  <si>
+    <t>To output values or print text in C#, it will add a new line for each method</t>
+  </si>
+  <si>
+    <t>Multi-line comment</t>
+  </si>
+  <si>
+    <t>Single-line comment</t>
+  </si>
+  <si>
+    <t>type variableName = value;</t>
+  </si>
+  <si>
+    <t>Variables</t>
+  </si>
+  <si>
+    <t>int myNum = 15; int myNum1;</t>
+  </si>
+  <si>
+    <t>const double PI = 3.14159265359;</t>
+  </si>
+  <si>
+    <t>char myLetter = 'D';</t>
+  </si>
+  <si>
+    <t>bool myBool = true; bool isSunny = false;</t>
+  </si>
+  <si>
+    <t>string myText = "Hello";</t>
+  </si>
+  <si>
+    <t>Example of  string</t>
+  </si>
+  <si>
+    <t>string name = "John"; or string myText='Text';</t>
+  </si>
+  <si>
+    <t>string myText = "text1"+"text2"</t>
+  </si>
+  <si>
+    <t>string first = "A "; string second = "C";string full = first + second;</t>
+  </si>
+  <si>
+    <t>int x = 5;  int x = 5, y = 6, z = 50; int x, y, z; x = y = z = 50;</t>
+  </si>
+  <si>
+    <t>Names can contain letters, digits and the underscore character (_)</t>
+  </si>
+  <si>
+    <t>Names must begin with a letter</t>
+  </si>
+  <si>
+    <t>Names should start with a lowercase letter and it cannot contain whitespace</t>
+  </si>
+  <si>
+    <t>Names are case sensitive ("myVar" and "myvar" are different variables)</t>
+  </si>
+  <si>
+    <t>Reserved words (like C# keywords, such as int or double) cannot be used as names</t>
+  </si>
+  <si>
+    <t>Rules for naming variables are:</t>
+  </si>
+  <si>
+    <t>long myNum = 15000000000L;</t>
+  </si>
+  <si>
+    <t>float myNum = 5.75F;float f1 = 35e3F;</t>
+  </si>
+  <si>
+    <t>double myDoubleNum = 5.99D;double d1 = 12E4D;</t>
+  </si>
+  <si>
+    <r>
+      <t>Explicit Casting</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (manually) - converting a larger type to a smaller size type</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Implicit Casting</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (automatically) - converting a smaller type to a larger type size</t>
+    </r>
+  </si>
+  <si>
+    <t>char -&gt; int -&gt; long -&gt; float -&gt; double Example: int myInt = 9; double myDouble = myInt;</t>
+  </si>
+  <si>
+    <t>double -&gt; float -&gt; long -&gt; int -&gt; char. Example: double myDouble = 9.78;
+int myInt = (int) myDouble;</t>
+  </si>
+  <si>
+    <t>Convert.ToDouble(12)</t>
+  </si>
+  <si>
+    <t>Convert.ToString(13)</t>
+  </si>
+  <si>
+    <t>double -&gt; int</t>
+  </si>
+  <si>
+    <t>int -&gt; double</t>
+  </si>
+  <si>
+    <t>int -&gt; string</t>
+  </si>
+  <si>
+    <t>Convert.ToString(false)</t>
+  </si>
+  <si>
+    <t>Convert.ToInt64(15.15D)</t>
+  </si>
+  <si>
+    <t>double-&gt;long</t>
+  </si>
+  <si>
+    <t>bool-&gt;string</t>
+  </si>
+  <si>
+    <t>Convert.ToInt32(12.57D)</t>
+  </si>
+  <si>
+    <t>ReadLine()</t>
+  </si>
+  <si>
+    <t>To get user input as string</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -631,8 +1094,86 @@
       <color rgb="FF232629"/>
       <name val="Inherit"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0077AA"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF999999"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFDD4A68"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF669900"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -657,8 +1198,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -666,20 +1213,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF04AA6D"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -694,8 +1248,41 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -973,378 +1560,503 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="44.7109375" customWidth="1"/>
     <col min="3" max="3" width="0.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="32.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="73.42578125" customWidth="1"/>
+    <col min="5" max="5" width="0.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" customWidth="1"/>
+    <col min="13" max="13" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:14">
       <c r="A1" s="4" t="s">
-        <v>44</v>
+        <v>119</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:5">
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="4" spans="1:5">
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="5" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B4" s="3"/>
       <c r="D4" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>128</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="I4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="20"/>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="2" t="s">
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" ht="4.5" customHeight="1">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="D8" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="2" t="s">
-        <v>37</v>
-      </c>
+      <c r="J8" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="2" t="s">
-        <v>35</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="I10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="4.5" customHeight="1">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="I13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="D14" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="D13" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="D14" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="B15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="G15" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="N15" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="D16" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="N16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="D17" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="N17" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="D18" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="19"/>
+      <c r="G21" s="14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="2" t="s">
+      <c r="B22" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="2" t="s">
+      <c r="B23" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="2" t="s">
+      <c r="B24" s="19"/>
+      <c r="G24" s="15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="2" t="s">
+      <c r="B25" s="19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="2" t="s">
+      <c r="B26" s="19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="D22" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="2"/>
-      <c r="D25" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="11" t="s">
+      <c r="B27" s="19" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="20"/>
+    </row>
+    <row r="29" spans="1:14" ht="51" customHeight="1">
+      <c r="A29" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="57" customHeight="1">
+      <c r="A30" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="19"/>
+      <c r="B31" s="19"/>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="2" t="s">
+      <c r="B32" s="19"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B33" s="19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="2" t="s">
+    <row r="34" spans="1:3">
+      <c r="A34" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B34" s="19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="2" t="s">
+    <row r="35" spans="1:3">
+      <c r="A35" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B35" s="25" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="3"/>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+        <v>156</v>
+      </c>
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="2" t="s">
-        <v>57</v>
+        <v>152</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
+        <v>155</v>
+      </c>
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="2" t="s">
-        <v>59</v>
+        <v>161</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
+        <v>154</v>
+      </c>
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" s="2" t="s">
-        <v>61</v>
+        <v>157</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
+        <v>160</v>
+      </c>
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" s="2" t="s">
-        <v>63</v>
+        <v>158</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>68</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="C40" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1353,15 +2065,15 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1372,70 +2084,82 @@
       <c r="B1" s="5"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>93</v>
+        <v>136</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2"/>
+        <v>137</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1483,16 +2207,16 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="5" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1506,163 +2230,163 @@
       <c r="C3" s="2"/>
       <c r="E3" s="2"/>
       <c r="G3" s="5" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2"/>
       <c r="C4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="G4" s="6" t="s">
-        <v>74</v>
+      <c r="G4" s="18" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2"/>
       <c r="C5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="G5" s="6"/>
+      <c r="G5" s="18"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2"/>
       <c r="C6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="G6" s="6"/>
+      <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2"/>
       <c r="C7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="G7" s="6"/>
+      <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="2"/>
       <c r="C8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="G8" s="6"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="2"/>
       <c r="C9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="G9" s="6"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="2"/>
-      <c r="G10" s="7" t="s">
-        <v>75</v>
+      <c r="G10" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2"/>
-      <c r="G11" s="7" t="b">
+      <c r="G11" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="25.5" customHeight="1">
       <c r="A12" s="2"/>
-      <c r="G12" s="8" t="s">
-        <v>76</v>
+      <c r="G12" s="7" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="2"/>
-      <c r="G13" s="9">
+      <c r="G13" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2"/>
-      <c r="G14" s="9">
+      <c r="G14" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2"/>
-      <c r="G15" s="9" t="s">
-        <v>77</v>
+      <c r="G15" s="8" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="2"/>
       <c r="G16" s="2" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="2"/>
       <c r="G17" s="2" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="13.5" customHeight="1">
       <c r="A18" s="2"/>
-      <c r="G18" s="8" t="s">
-        <v>80</v>
+      <c r="G18" s="7" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="18.75" customHeight="1">
       <c r="A19" s="2"/>
-      <c r="G19" s="9" t="s">
-        <v>81</v>
+      <c r="G19" s="8" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="2"/>
-      <c r="G20" s="9" t="s">
-        <v>82</v>
+      <c r="G20" s="8" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="20.25" customHeight="1">
       <c r="A21" s="2"/>
-      <c r="G21" s="9" t="s">
-        <v>83</v>
+      <c r="G21" s="8" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" s="4"/>
-      <c r="G22" s="9" t="s">
-        <v>84</v>
+      <c r="G22" s="8" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15" customHeight="1">
-      <c r="G23" s="9" t="s">
-        <v>85</v>
+      <c r="G23" s="8" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="24.95" customHeight="1">
-      <c r="G24" s="9" t="s">
-        <v>86</v>
+      <c r="G24" s="8" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="24.95" customHeight="1">
-      <c r="G25" s="9" t="s">
-        <v>87</v>
+      <c r="G25" s="8" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="24.95" customHeight="1">
-      <c r="G26" s="9" t="s">
-        <v>88</v>
+      <c r="G26" s="8" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="24.95" customHeight="1">
-      <c r="G27" s="10" t="s">
-        <v>89</v>
+      <c r="G27" s="9" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="24.95" customHeight="1">
-      <c r="G28" s="8" t="s">
-        <v>90</v>
+      <c r="G28" s="7" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="24.95" customHeight="1">
-      <c r="G29" s="9" t="s">
-        <v>91</v>
+      <c r="G29" s="8" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="24.95" customHeight="1">
-      <c r="G30" s="9" t="s">
-        <v>92</v>
+      <c r="G30" s="8" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1671,4 +2395,83 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="54.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="17"/>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="17"/>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="17"/>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="17"/>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="17"/>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" s="17"/>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="17"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated tab for data-structures
</commit_message>
<xml_diff>
--- a/Csharp-cheatsheet-acoptexlt.xlsx
+++ b/Csharp-cheatsheet-acoptexlt.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D594BD0-A627-4284-B159-88D693A8C8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="2" r:id="rId1"/>
@@ -23,12 +24,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B22" authorId="0" shapeId="0">
+    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="167">
   <si>
     <t>string.Equals("Text")</t>
   </si>
@@ -1054,12 +1055,21 @@
   </si>
   <si>
     <t>To get user input as string</t>
+  </si>
+  <si>
+    <t>Arrays</t>
+  </si>
+  <si>
+    <t>Lists</t>
+  </si>
+  <si>
+    <t>Dictionaries</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="17">
     <font>
       <sz val="11"/>
@@ -1227,9 +1237,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1262,11 +1271,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1280,6 +1284,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1560,13 +1567,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
@@ -1574,7 +1581,7 @@
   <cols>
     <col min="1" max="1" width="26.7109375" customWidth="1"/>
     <col min="2" max="2" width="44.7109375" customWidth="1"/>
-    <col min="3" max="3" width="0.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="0.42578125" customWidth="1"/>
     <col min="4" max="4" width="73.42578125" customWidth="1"/>
     <col min="5" max="5" width="0.5703125" customWidth="1"/>
     <col min="6" max="6" width="22.140625" customWidth="1"/>
@@ -1582,226 +1589,223 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="D4" s="5" t="s">
+      <c r="B4" s="2"/>
+      <c r="D4" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="I4" s="5" t="s">
+      <c r="G4" s="4"/>
+      <c r="I4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="20"/>
+      <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="D7" s="2" t="s">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="D7" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="D8" s="2" t="s">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="D8" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="D9" s="2" t="s">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="D9" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="D10" s="2" t="s">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="D10" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="I10" s="2" t="s">
+      <c r="G10" s="1"/>
+      <c r="I10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="D11" s="2" t="s">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="D11" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="D12" s="2" t="s">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="D12" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="4.5" customHeight="1">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="D14" s="5" t="s">
+      <c r="B14" s="2"/>
+      <c r="D14" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="M14" s="5" t="s">
+      <c r="M14" s="4" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="G15" s="12" t="s">
+      <c r="B15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="G15" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="M15" s="1" t="s">
         <v>121</v>
       </c>
       <c r="N15" t="s">
@@ -1809,17 +1813,17 @@
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="D16" s="5" t="s">
+      <c r="B16" s="1"/>
+      <c r="D16" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="M16" s="2" t="s">
+      <c r="M16" s="1" t="s">
         <v>122</v>
       </c>
       <c r="N16" t="s">
@@ -1827,17 +1831,17 @@
       </c>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="D17" s="11" t="s">
+      <c r="B17" s="1"/>
+      <c r="D17" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="M17" s="1" t="s">
         <v>162</v>
       </c>
       <c r="N17" t="s">
@@ -1845,213 +1849,213 @@
       </c>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="D18" s="5" t="s">
+      <c r="B18" s="1"/>
+      <c r="D18" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="G18" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="M18" s="5" t="s">
+      <c r="M18" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="M19" s="2" t="s">
+      <c r="M19" s="1" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="M20" s="2"/>
+      <c r="M20" s="1"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="G21" s="14" t="s">
+      <c r="B21" s="1"/>
+      <c r="G21" s="13" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="G22" s="14" t="s">
+      <c r="G22" s="13" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="G23" s="13" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="G24" s="15" t="s">
+      <c r="B24" s="1"/>
+      <c r="G24" s="14" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="1" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="1" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="1" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:14">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B28" s="20"/>
+      <c r="B28" s="2"/>
     </row>
     <row r="29" spans="1:14" ht="51" customHeight="1">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="17" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="57" customHeight="1">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="20" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:14">
-      <c r="A31" s="19"/>
-      <c r="B31" s="19"/>
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
     </row>
     <row r="32" spans="1:14">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B32" s="19"/>
+      <c r="B32" s="1"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="19" t="s">
+      <c r="A34" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="25" t="s">
+      <c r="A35" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="25" t="s">
+      <c r="B35" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C36" s="2"/>
+      <c r="C36" s="1"/>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C37" s="2"/>
+      <c r="C37" s="1"/>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C38" s="2"/>
+      <c r="C38" s="1"/>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C39" s="2"/>
+      <c r="C39" s="1"/>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C40" s="2"/>
+      <c r="C40" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2061,7 +2065,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -2078,88 +2082,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="1"/>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="1"/>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="1"/>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2167,24 +2171,36 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -2206,186 +2222,186 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="A2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="G3" s="5" t="s">
+      <c r="A3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="G3" s="4" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="G4" s="18" t="s">
+      <c r="A4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="G4" s="22" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="G5" s="18"/>
+      <c r="A5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="G6" s="18"/>
+      <c r="A6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="G6" s="22"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="G7" s="18"/>
+      <c r="A7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="G7" s="22"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="G8" s="18"/>
+      <c r="A8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="G8" s="22"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="2"/>
-      <c r="C9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="G9" s="18"/>
+      <c r="A9" s="1"/>
+      <c r="C9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="G9" s="22"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="2"/>
-      <c r="G10" s="6" t="s">
+      <c r="A10" s="1"/>
+      <c r="G10" s="5" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="2"/>
-      <c r="G11" s="6" t="b">
+      <c r="A11" s="1"/>
+      <c r="G11" s="5" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A12" s="2"/>
-      <c r="G12" s="7" t="s">
+      <c r="A12" s="1"/>
+      <c r="G12" s="6" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="2"/>
-      <c r="G13" s="8">
+      <c r="A13" s="1"/>
+      <c r="G13" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="2"/>
-      <c r="G14" s="8">
+      <c r="A14" s="1"/>
+      <c r="G14" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="2"/>
-      <c r="G15" s="8" t="s">
+      <c r="A15" s="1"/>
+      <c r="G15" s="7" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="2"/>
-      <c r="G16" s="2" t="s">
+      <c r="A16" s="1"/>
+      <c r="G16" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="2"/>
-      <c r="G17" s="2" t="s">
+      <c r="A17" s="1"/>
+      <c r="G17" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A18" s="2"/>
-      <c r="G18" s="7" t="s">
+      <c r="A18" s="1"/>
+      <c r="G18" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A19" s="2"/>
-      <c r="G19" s="8" t="s">
+      <c r="A19" s="1"/>
+      <c r="G19" s="7" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="2"/>
-      <c r="G20" s="8" t="s">
+      <c r="A20" s="1"/>
+      <c r="G20" s="7" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="20.25" customHeight="1">
-      <c r="A21" s="2"/>
-      <c r="G21" s="8" t="s">
+      <c r="A21" s="1"/>
+      <c r="G21" s="7" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A22" s="4"/>
-      <c r="G22" s="8" t="s">
+      <c r="A22" s="3"/>
+      <c r="G22" s="7" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15" customHeight="1">
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="7" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="24.95" customHeight="1">
-      <c r="G24" s="8" t="s">
+      <c r="G24" s="7" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="24.95" customHeight="1">
-      <c r="G25" s="8" t="s">
+      <c r="G25" s="7" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="24.95" customHeight="1">
-      <c r="G26" s="8" t="s">
+      <c r="G26" s="7" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="24.95" customHeight="1">
-      <c r="G27" s="9" t="s">
+      <c r="G27" s="8" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="24.95" customHeight="1">
-      <c r="G28" s="7" t="s">
+      <c r="G28" s="6" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="24.95" customHeight="1">
-      <c r="G29" s="8" t="s">
+      <c r="G29" s="7" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="24.95" customHeight="1">
-      <c r="G30" s="8" t="s">
+      <c r="G30" s="7" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2398,7 +2414,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -2414,62 +2430,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="17"/>
+      <c r="B2" s="16"/>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="17"/>
+      <c r="B3" s="16"/>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="16"/>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="17"/>
+      <c r="B5" s="16"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="17"/>
+      <c r="B6" s="16"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="17"/>
+      <c r="B7" s="16"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="B8" s="17"/>
+      <c r="B8" s="16"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1"/>
-    <hyperlink ref="A4" r:id="rId2"/>
-    <hyperlink ref="A5" r:id="rId3"/>
-    <hyperlink ref="A2" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="A2" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>

</xml_diff>